<commit_message>
Some changes in AAI
</commit_message>
<xml_diff>
--- a/malf.xlsx
+++ b/malf.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="6">
   <si>
     <t>normal</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>noAnswer</t>
+  </si>
+  <si>
+    <t>unrelized</t>
   </si>
 </sst>
 </file>
@@ -391,13 +394,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAF0E20E-E4D8-9B45-9C94-E89B574F109C}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,13 +416,16 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="b">
         <v>1</v>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -430,10 +436,13 @@
       <c r="E2" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -442,21 +451,24 @@
         <v>0</v>
       </c>
       <c r="D3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="b">
         <v>1</v>
       </c>
       <c r="B4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -464,10 +476,13 @@
       <c r="E4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -476,13 +491,16 @@
         <v>0</v>
       </c>
       <c r="D5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="b">
         <v>1</v>
       </c>
@@ -498,8 +516,11 @@
       <c r="E6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="b">
         <v>1</v>
       </c>
@@ -515,8 +536,11 @@
       <c r="E7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="b">
         <v>1</v>
       </c>
@@ -532,8 +556,11 @@
       <c r="E8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="b">
         <v>1</v>
       </c>
@@ -549,8 +576,11 @@
       <c r="E9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="b">
         <v>1</v>
       </c>
@@ -566,8 +596,11 @@
       <c r="E10" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="b">
         <v>1</v>
       </c>
@@ -583,8 +616,11 @@
       <c r="E11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="b">
         <v>1</v>
       </c>
@@ -600,8 +636,11 @@
       <c r="E12" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="b">
         <v>1</v>
       </c>
@@ -615,10 +654,13 @@
         <v>0</v>
       </c>
       <c r="E13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>1</v>
+      </c>
+      <c r="F13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="b">
         <v>0</v>
       </c>
@@ -632,18 +674,21 @@
         <v>1</v>
       </c>
       <c r="E14" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="F14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="b">
         <v>1</v>
       </c>
       <c r="B15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -651,10 +696,13 @@
       <c r="E15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16" t="b">
         <v>0</v>
@@ -663,21 +711,24 @@
         <v>0</v>
       </c>
       <c r="D16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="F16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="b">
         <v>1</v>
       </c>
       <c r="B17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" t="b">
         <v>0</v>
@@ -685,8 +736,11 @@
       <c r="E17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="b">
         <v>1</v>
       </c>
@@ -702,8 +756,11 @@
       <c r="E18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="b">
         <v>1</v>
       </c>
@@ -719,16 +776,19 @@
       <c r="E19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="b">
         <v>1</v>
       </c>
       <c r="B20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -736,10 +796,13 @@
       <c r="E20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B21" t="b">
         <v>0</v>
@@ -748,21 +811,24 @@
         <v>0</v>
       </c>
       <c r="D21" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>0</v>
+      </c>
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="b">
         <v>1</v>
       </c>
       <c r="B22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" t="b">
         <v>0</v>
@@ -770,8 +836,11 @@
       <c r="E22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="b">
         <v>1</v>
       </c>
@@ -787,8 +856,11 @@
       <c r="E23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="b">
         <v>1</v>
       </c>
@@ -804,16 +876,19 @@
       <c r="E24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="b">
         <v>1</v>
       </c>
       <c r="B25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" t="b">
         <v>0</v>
@@ -821,10 +896,13 @@
       <c r="E25" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B26" t="b">
         <v>0</v>
@@ -833,10 +911,13 @@
         <v>0</v>
       </c>
       <c r="D26" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F26" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>